<commit_message>
add data tables and export buttons
</commit_message>
<xml_diff>
--- a/c_maridadi/Churamiti maridadi.xlsx
+++ b/c_maridadi/Churamiti maridadi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophliedtke/Documents/git_projects/extinct/c_maridadi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/L9HRVWMTX/Nextcloud_eed/tanzania/Ukaguru Arthroleptis paper and survey data/extinction estimations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D3110-E085-0E4A-A8AC-04CEE2129C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B691BFF0-EF8B-9B41-9BE7-F3D6A7A3FC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="760" windowWidth="19500" windowHeight="16820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="5180" windowWidth="18540" windowHeight="17800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threats" sheetId="5" r:id="rId1"/>
@@ -21,15 +21,13 @@
     <sheet name="export" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1768,7 +1766,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>5.9100000000000041E-2</c:v>
+                    <c:v>0.22100000000000009</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1780,7 +1778,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>3.839999999999999E-2</c:v>
+                    <c:v>0.10899999999999999</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1853,7 +1851,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.94089999999999996</c:v>
+                  <c:v>0.67899999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2559,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2699,13 +2697,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="86">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="C13" s="86">
-        <v>0.97</v>
+        <v>0.7</v>
       </c>
       <c r="D13" s="86">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>56</v>
@@ -2805,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4395,8 +4393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4618,28 +4616,28 @@
         <v>0.01</v>
       </c>
       <c r="C12" s="84">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="D12" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="84">
         <v>0.05</v>
       </c>
-      <c r="E12" s="84">
-        <v>0.7</v>
-      </c>
       <c r="F12" s="84">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="G12" s="84">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="H12" s="84">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="I12" s="84">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="J12" s="84">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="K12" s="84"/>
       <c r="L12" s="84"/>
@@ -4706,31 +4704,31 @@
         <v>2002</v>
       </c>
       <c r="B15" s="84">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="C15" s="84">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="D15" s="84">
+        <v>0.03</v>
+      </c>
+      <c r="E15" s="84">
         <v>0.6</v>
       </c>
-      <c r="E15" s="84">
-        <v>0.9</v>
-      </c>
       <c r="F15" s="84">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="G15" s="84">
+        <v>0.8</v>
+      </c>
+      <c r="H15" s="84">
         <v>0.99</v>
       </c>
-      <c r="H15" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I15" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J15" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K15" s="84"/>
       <c r="L15" s="84"/>
@@ -4741,381 +4739,361 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="84">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B16" s="84">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="84">
+        <v>0.08</v>
+      </c>
+      <c r="D16" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F16" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G16" s="84">
         <v>0.8</v>
       </c>
-      <c r="C16" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D16" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E16" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F16" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G16" s="84">
+      <c r="H16" s="84">
         <v>0.99</v>
       </c>
-      <c r="H16" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I16" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J16" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K16" s="84"/>
       <c r="L16" s="84"/>
       <c r="N16" s="25" t="str">
-        <f>IF(OR(H16&gt;I16,I16&gt;J16,E16&gt;F16,F16&gt;G16,B16&gt;C16,C16&gt;D16),"lower bound, best est, upper bound are not in correct order",IF(OR(B16&lt;0,B16&gt;1,C16&lt;0,C16&gt;1,D16&lt;0,D16&gt;1,E16&lt;0,E16&gt;1,F16&lt;0,F16&gt;1,G16&lt;0,G16&gt;1,H16&lt;0,H16&gt;1,I16&lt;0,I16&gt;1,J16&lt;0,J16&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" ref="N16:N25" si="1">IF(OR(H16&gt;I16,I16&gt;J16,E16&gt;F16,F16&gt;G16,B16&gt;C16,C16&gt;D16),"lower bound, best est, upper bound are not in correct order",IF(OR(B16&lt;0,B16&gt;1,C16&lt;0,C16&gt;1,D16&lt;0,D16&gt;1,E16&lt;0,E16&gt;1,F16&lt;0,F16&gt;1,G16&lt;0,G16&gt;1,H16&lt;0,H16&gt;1,I16&lt;0,I16&gt;1,J16&lt;0,J16&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
         <v>ok</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="84">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="B17" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="84">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="84">
+        <v>0.4</v>
+      </c>
+      <c r="F17" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="H17" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="I17" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="J17" s="84">
         <v>0.8</v>
-      </c>
-      <c r="C17" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D17" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E17" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F17" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G17" s="84">
-        <v>0.99</v>
-      </c>
-      <c r="H17" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="84">
-        <v>0.6</v>
-      </c>
-      <c r="J17" s="84">
-        <v>0.7</v>
       </c>
       <c r="K17" s="84"/>
       <c r="L17" s="84"/>
       <c r="N17" s="25" t="str">
-        <f>IF(OR(H17&gt;I17,I17&gt;J17,E17&gt;F17,F17&gt;G17,B17&gt;C17,C17&gt;D17),"lower bound, best est, upper bound are not in correct order",IF(OR(B17&lt;0,B17&gt;1,C17&lt;0,C17&gt;1,D17&lt;0,D17&gt;1,E17&lt;0,E17&gt;1,F17&lt;0,F17&gt;1,G17&lt;0,G17&gt;1,H17&lt;0,H17&gt;1,I17&lt;0,I17&gt;1,J17&lt;0,J17&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="84">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="B18" s="84">
+        <v>0.03</v>
+      </c>
+      <c r="C18" s="84">
+        <v>0.04</v>
+      </c>
+      <c r="D18" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F18" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G18" s="84">
         <v>0.8</v>
       </c>
-      <c r="C18" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D18" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E18" s="84">
-        <v>0.4</v>
-      </c>
-      <c r="F18" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="84">
-        <v>0.6</v>
-      </c>
       <c r="H18" s="84">
-        <v>0.5</v>
+        <v>0.99</v>
       </c>
       <c r="I18" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J18" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K18" s="84"/>
       <c r="L18" s="84"/>
       <c r="N18" s="25" t="str">
-        <f>IF(OR(H18&gt;I18,I18&gt;J18,E18&gt;F18,F18&gt;G18,B18&gt;C18,C18&gt;D18),"lower bound, best est, upper bound are not in correct order",IF(OR(B18&lt;0,B18&gt;1,C18&lt;0,C18&gt;1,D18&lt;0,D18&gt;1,E18&lt;0,E18&gt;1,F18&lt;0,F18&gt;1,G18&lt;0,G18&gt;1,H18&lt;0,H18&gt;1,I18&lt;0,I18&gt;1,J18&lt;0,J18&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="84">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B19" s="84">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="C19" s="84">
-        <v>0.5</v>
+        <v>0.08</v>
       </c>
       <c r="D19" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="84">
         <v>0.6</v>
       </c>
-      <c r="E19" s="84">
-        <v>0.9</v>
-      </c>
       <c r="F19" s="84">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="G19" s="84">
+        <v>0.8</v>
+      </c>
+      <c r="H19" s="84">
         <v>0.99</v>
       </c>
-      <c r="H19" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I19" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J19" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="84"/>
       <c r="N19" s="25" t="str">
-        <f>IF(OR(H19&gt;I19,I19&gt;J19,E19&gt;F19,F19&gt;G19,B19&gt;C19,C19&gt;D19),"lower bound, best est, upper bound are not in correct order",IF(OR(B19&lt;0,B19&gt;1,C19&lt;0,C19&gt;1,D19&lt;0,D19&gt;1,E19&lt;0,E19&gt;1,F19&lt;0,F19&gt;1,G19&lt;0,G19&gt;1,H19&lt;0,H19&gt;1,I19&lt;0,I19&gt;1,J19&lt;0,J19&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="84">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B20" s="84">
+        <v>0.01</v>
+      </c>
+      <c r="C20" s="84">
+        <v>0.02</v>
+      </c>
+      <c r="D20" s="84">
+        <v>0.05</v>
+      </c>
+      <c r="E20" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G20" s="84">
         <v>0.8</v>
       </c>
-      <c r="C20" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D20" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E20" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F20" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G20" s="84">
+      <c r="H20" s="84">
         <v>0.99</v>
       </c>
-      <c r="H20" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I20" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J20" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K20" s="84"/>
       <c r="L20" s="84"/>
       <c r="N20" s="25" t="str">
-        <f>IF(OR(H20&gt;I20,I20&gt;J20,E20&gt;F20,F20&gt;G20,B20&gt;C20,C20&gt;D20),"lower bound, best est, upper bound are not in correct order",IF(OR(B20&lt;0,B20&gt;1,C20&lt;0,C20&gt;1,D20&lt;0,D20&gt;1,E20&lt;0,E20&gt;1,F20&lt;0,F20&gt;1,G20&lt;0,G20&gt;1,H20&lt;0,H20&gt;1,I20&lt;0,I20&gt;1,J20&lt;0,J20&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="84">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="B21" s="84">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="C21" s="84">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D21" s="84">
+        <v>0.15</v>
+      </c>
+      <c r="E21" s="84">
         <v>0.6</v>
       </c>
-      <c r="E21" s="84">
-        <v>0.9</v>
-      </c>
       <c r="F21" s="84">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="G21" s="84">
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="84">
         <v>0.99</v>
       </c>
-      <c r="H21" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I21" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J21" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K21" s="84"/>
       <c r="L21" s="84"/>
       <c r="N21" s="25" t="str">
-        <f>IF(OR(H21&gt;I21,I21&gt;J21,E21&gt;F21,F21&gt;G21,B21&gt;C21,C21&gt;D21),"lower bound, best est, upper bound are not in correct order",IF(OR(B21&lt;0,B21&gt;1,C21&lt;0,C21&gt;1,D21&lt;0,D21&gt;1,E21&lt;0,E21&gt;1,F21&lt;0,F21&gt;1,G21&lt;0,G21&gt;1,H21&lt;0,H21&gt;1,I21&lt;0,I21&gt;1,J21&lt;0,J21&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="84">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B22" s="84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C22" s="84">
+        <v>0.12</v>
+      </c>
+      <c r="D22" s="84">
+        <v>0.15</v>
+      </c>
+      <c r="E22" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F22" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G22" s="84">
         <v>0.8</v>
       </c>
-      <c r="C22" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D22" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E22" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F22" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G22" s="84">
+      <c r="H22" s="84">
         <v>0.99</v>
       </c>
-      <c r="H22" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I22" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J22" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K22" s="84"/>
       <c r="L22" s="84"/>
       <c r="N22" s="25" t="str">
-        <f>IF(OR(H22&gt;I22,I22&gt;J22,E22&gt;F22,F22&gt;G22,B22&gt;C22,C22&gt;D22),"lower bound, best est, upper bound are not in correct order",IF(OR(B22&lt;0,B22&gt;1,C22&lt;0,C22&gt;1,D22&lt;0,D22&gt;1,E22&lt;0,E22&gt;1,F22&lt;0,F22&gt;1,G22&lt;0,G22&gt;1,H22&lt;0,H22&gt;1,I22&lt;0,I22&gt;1,J22&lt;0,J22&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="84">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B23" s="84">
+        <v>0.15</v>
+      </c>
+      <c r="C23" s="84">
+        <v>0.17</v>
+      </c>
+      <c r="D23" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F23" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G23" s="84">
         <v>0.8</v>
       </c>
-      <c r="C23" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D23" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E23" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F23" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G23" s="84">
+      <c r="H23" s="84">
         <v>0.99</v>
       </c>
-      <c r="H23" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I23" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J23" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K23" s="84"/>
       <c r="L23" s="84"/>
       <c r="N23" s="25" t="str">
-        <f>IF(OR(H23&gt;I23,I23&gt;J23,E23&gt;F23,F23&gt;G23,B23&gt;C23,C23&gt;D23),"lower bound, best est, upper bound are not in correct order",IF(OR(B23&lt;0,B23&gt;1,C23&lt;0,C23&gt;1,D23&lt;0,D23&gt;1,E23&lt;0,E23&gt;1,F23&lt;0,F23&gt;1,G23&lt;0,G23&gt;1,H23&lt;0,H23&gt;1,I23&lt;0,I23&gt;1,J23&lt;0,J23&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="84">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B24" s="84">
+        <v>0.15</v>
+      </c>
+      <c r="C24" s="84">
+        <v>0.17</v>
+      </c>
+      <c r="D24" s="84">
+        <v>0.25</v>
+      </c>
+      <c r="E24" s="84">
+        <v>0.6</v>
+      </c>
+      <c r="F24" s="84">
+        <v>0.7</v>
+      </c>
+      <c r="G24" s="84">
         <v>0.8</v>
       </c>
-      <c r="C24" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D24" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E24" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F24" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G24" s="84">
+      <c r="H24" s="84">
         <v>0.99</v>
       </c>
-      <c r="H24" s="84">
-        <v>0.5</v>
-      </c>
       <c r="I24" s="84">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="J24" s="84">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="K24" s="84"/>
       <c r="L24" s="84"/>
       <c r="N24" s="25" t="str">
-        <f>IF(OR(H24&gt;I24,I24&gt;J24,E24&gt;F24,F24&gt;G24,B24&gt;C24,C24&gt;D24),"lower bound, best est, upper bound are not in correct order",IF(OR(B24&lt;0,B24&gt;1,C24&lt;0,C24&gt;1,D24&lt;0,D24&gt;1,E24&lt;0,E24&gt;1,F24&lt;0,F24&gt;1,G24&lt;0,G24&gt;1,H24&lt;0,H24&gt;1,I24&lt;0,I24&gt;1,J24&lt;0,J24&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="84">
-        <v>2024</v>
-      </c>
-      <c r="B25" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="C25" s="84">
-        <v>0.8</v>
-      </c>
-      <c r="D25" s="84">
-        <v>0.95</v>
-      </c>
-      <c r="E25" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="F25" s="84">
-        <v>0.9</v>
-      </c>
-      <c r="G25" s="84">
-        <v>0.99</v>
-      </c>
-      <c r="H25" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="I25" s="84">
-        <v>0.6</v>
-      </c>
-      <c r="J25" s="84">
-        <v>0.7</v>
-      </c>
+      <c r="A25" s="84"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
       <c r="K25" s="84"/>
       <c r="L25" s="84"/>
       <c r="N25" s="25" t="str">
-        <f>IF(OR(H25&gt;I25,I25&gt;J25,E25&gt;F25,F25&gt;G25,B25&gt;C25,C25&gt;D25),"lower bound, best est, upper bound are not in correct order",IF(OR(B25&lt;0,B25&gt;1,C25&lt;0,C25&gt;1,D25&lt;0,D25&gt;1,E25&lt;0,E25&gt;1,F25&lt;0,F25&gt;1,G25&lt;0,G25&gt;1,H25&lt;0,H25&gt;1,I25&lt;0,I25&gt;1,J25&lt;0,J25&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" si="1"/>
         <v>ok</v>
       </c>
     </row>
@@ -6087,7 +6065,7 @@
       <c r="K79" s="84"/>
       <c r="L79" s="84"/>
       <c r="N79" s="25" t="str">
-        <f t="shared" ref="N79:N125" si="1">IF(OR(H79&gt;I79,I79&gt;J79,E79&gt;F79,F79&gt;G79,B79&gt;C79,C79&gt;D79),"lower bound, best est, upper bound are not in correct order",IF(OR(B79&lt;0,B79&gt;1,C79&lt;0,C79&gt;1,D79&lt;0,D79&gt;1,E79&lt;0,E79&gt;1,F79&lt;0,F79&gt;1,G79&lt;0,G79&gt;1,H79&lt;0,H79&gt;1,I79&lt;0,I79&gt;1,J79&lt;0,J79&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
+        <f t="shared" ref="N79:N125" si="2">IF(OR(H79&gt;I79,I79&gt;J79,E79&gt;F79,F79&gt;G79,B79&gt;C79,C79&gt;D79),"lower bound, best est, upper bound are not in correct order",IF(OR(B79&lt;0,B79&gt;1,C79&lt;0,C79&gt;1,D79&lt;0,D79&gt;1,E79&lt;0,E79&gt;1,F79&lt;0,F79&gt;1,G79&lt;0,G79&gt;1,H79&lt;0,H79&gt;1,I79&lt;0,I79&gt;1,J79&lt;0,J79&gt;1),"Probabilities must be between 0 and 1","ok"))</f>
         <v>ok</v>
       </c>
     </row>
@@ -6105,7 +6083,7 @@
       <c r="K80" s="84"/>
       <c r="L80" s="84"/>
       <c r="N80" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6123,7 +6101,7 @@
       <c r="K81" s="84"/>
       <c r="L81" s="84"/>
       <c r="N81" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6141,7 +6119,7 @@
       <c r="K82" s="84"/>
       <c r="L82" s="84"/>
       <c r="N82" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6159,7 +6137,7 @@
       <c r="K83" s="84"/>
       <c r="L83" s="84"/>
       <c r="N83" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6177,7 +6155,7 @@
       <c r="K84" s="84"/>
       <c r="L84" s="84"/>
       <c r="N84" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6195,7 +6173,7 @@
       <c r="K85" s="84"/>
       <c r="L85" s="84"/>
       <c r="N85" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6213,7 +6191,7 @@
       <c r="K86" s="84"/>
       <c r="L86" s="84"/>
       <c r="N86" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6231,7 +6209,7 @@
       <c r="K87" s="84"/>
       <c r="L87" s="84"/>
       <c r="N87" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6249,7 +6227,7 @@
       <c r="K88" s="84"/>
       <c r="L88" s="84"/>
       <c r="N88" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6267,7 +6245,7 @@
       <c r="K89" s="84"/>
       <c r="L89" s="84"/>
       <c r="N89" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6285,7 +6263,7 @@
       <c r="K90" s="84"/>
       <c r="L90" s="84"/>
       <c r="N90" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6303,7 +6281,7 @@
       <c r="K91" s="84"/>
       <c r="L91" s="84"/>
       <c r="N91" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6321,7 +6299,7 @@
       <c r="K92" s="84"/>
       <c r="L92" s="84"/>
       <c r="N92" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6339,7 +6317,7 @@
       <c r="K93" s="84"/>
       <c r="L93" s="84"/>
       <c r="N93" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6357,7 +6335,7 @@
       <c r="K94" s="84"/>
       <c r="L94" s="84"/>
       <c r="N94" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6375,7 +6353,7 @@
       <c r="K95" s="84"/>
       <c r="L95" s="84"/>
       <c r="N95" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6393,7 +6371,7 @@
       <c r="K96" s="84"/>
       <c r="L96" s="84"/>
       <c r="N96" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6411,7 +6389,7 @@
       <c r="K97" s="84"/>
       <c r="L97" s="84"/>
       <c r="N97" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6429,7 +6407,7 @@
       <c r="K98" s="84"/>
       <c r="L98" s="84"/>
       <c r="N98" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6447,7 +6425,7 @@
       <c r="K99" s="84"/>
       <c r="L99" s="84"/>
       <c r="N99" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6465,7 +6443,7 @@
       <c r="K100" s="84"/>
       <c r="L100" s="84"/>
       <c r="N100" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6483,7 +6461,7 @@
       <c r="K101" s="84"/>
       <c r="L101" s="84"/>
       <c r="N101" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6501,7 +6479,7 @@
       <c r="K102" s="84"/>
       <c r="L102" s="84"/>
       <c r="N102" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6519,7 +6497,7 @@
       <c r="K103" s="84"/>
       <c r="L103" s="84"/>
       <c r="N103" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6537,7 +6515,7 @@
       <c r="K104" s="84"/>
       <c r="L104" s="84"/>
       <c r="N104" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6555,7 +6533,7 @@
       <c r="K105" s="84"/>
       <c r="L105" s="84"/>
       <c r="N105" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6573,7 +6551,7 @@
       <c r="K106" s="84"/>
       <c r="L106" s="84"/>
       <c r="N106" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6591,7 +6569,7 @@
       <c r="K107" s="84"/>
       <c r="L107" s="84"/>
       <c r="N107" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6609,7 +6587,7 @@
       <c r="K108" s="84"/>
       <c r="L108" s="84"/>
       <c r="N108" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6627,7 +6605,7 @@
       <c r="K109" s="84"/>
       <c r="L109" s="84"/>
       <c r="N109" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6645,7 +6623,7 @@
       <c r="K110" s="84"/>
       <c r="L110" s="84"/>
       <c r="N110" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6663,7 +6641,7 @@
       <c r="K111" s="84"/>
       <c r="L111" s="84"/>
       <c r="N111" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6681,7 +6659,7 @@
       <c r="K112" s="84"/>
       <c r="L112" s="84"/>
       <c r="N112" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6699,7 +6677,7 @@
       <c r="K113" s="84"/>
       <c r="L113" s="84"/>
       <c r="N113" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6717,7 +6695,7 @@
       <c r="K114" s="84"/>
       <c r="L114" s="84"/>
       <c r="N114" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6735,7 +6713,7 @@
       <c r="K115" s="84"/>
       <c r="L115" s="84"/>
       <c r="N115" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6753,7 +6731,7 @@
       <c r="K116" s="84"/>
       <c r="L116" s="84"/>
       <c r="N116" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6771,7 +6749,7 @@
       <c r="K117" s="84"/>
       <c r="L117" s="84"/>
       <c r="N117" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6789,7 +6767,7 @@
       <c r="K118" s="84"/>
       <c r="L118" s="84"/>
       <c r="N118" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6807,7 +6785,7 @@
       <c r="K119" s="84"/>
       <c r="L119" s="84"/>
       <c r="N119" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6825,7 +6803,7 @@
       <c r="K120" s="84"/>
       <c r="L120" s="84"/>
       <c r="N120" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6843,7 +6821,7 @@
       <c r="K121" s="84"/>
       <c r="L121" s="84"/>
       <c r="N121" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6861,7 +6839,7 @@
       <c r="K122" s="84"/>
       <c r="L122" s="84"/>
       <c r="N122" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6879,7 +6857,7 @@
       <c r="K123" s="84"/>
       <c r="L123" s="84"/>
       <c r="N123" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6897,7 +6875,7 @@
       <c r="K124" s="84"/>
       <c r="L124" s="84"/>
       <c r="N124" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6915,7 +6893,7 @@
       <c r="K125" s="84"/>
       <c r="L125" s="84"/>
       <c r="N125" s="25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
     </row>
@@ -6945,7 +6923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -7060,15 +7038,15 @@
       </c>
       <c r="C4" s="51">
         <f>Threats!B12*Threats!B13</f>
-        <v>0.90249999999999997</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D4" s="51">
         <f>Threats!C12*Threats!C13</f>
-        <v>0.94089999999999996</v>
+        <v>0.67899999999999994</v>
       </c>
       <c r="E4" s="51">
         <f>Threats!D12*Threats!D13</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F4" s="94" t="s">
         <v>77</v>
@@ -7115,7 +7093,7 @@
     <row r="10" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D10" s="83">
         <f>AVERAGE(D4:D5)</f>
-        <v>0.89544999999999997</v>
+        <v>0.76449999999999996</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -7146,19 +7124,19 @@
     <row r="13" spans="2:10" ht="19" x14ac:dyDescent="0.2">
       <c r="B13" s="69">
         <f>E4-C4</f>
-        <v>9.7500000000000031E-2</v>
+        <v>0.33000000000000007</v>
       </c>
       <c r="C13" s="63">
         <f>1/(B13+0.01)</f>
-        <v>9.3023255813953458</v>
+        <v>2.9411764705882346</v>
       </c>
       <c r="D13" s="63">
         <f>C13*D4</f>
-        <v>8.7525581395348802</v>
+        <v>1.9970588235294111</v>
       </c>
       <c r="E13" s="70">
         <f>D15/C15</f>
-        <v>0.90141818181818167</v>
+        <v>0.80012499999999986</v>
       </c>
       <c r="G13" s="123"/>
       <c r="H13" s="124"/>
@@ -7199,11 +7177,11 @@
       <c r="B15" s="73"/>
       <c r="C15" s="74">
         <f>SUM(C13:C14)</f>
-        <v>16.44518272425249</v>
+        <v>10.084033613445378</v>
       </c>
       <c r="D15" s="74">
         <f>SUM(D13:D14)</f>
-        <v>14.823986710963451</v>
+        <v>8.0684873949579821</v>
       </c>
       <c r="E15" s="62"/>
       <c r="G15" s="123"/>
@@ -7245,7 +7223,7 @@
       </c>
       <c r="H17" s="58">
         <f>D4-C4</f>
-        <v>3.839999999999999E-2</v>
+        <v>0.10899999999999999</v>
       </c>
       <c r="I17" s="55">
         <f>$C$8</f>
@@ -7258,19 +7236,19 @@
     <row r="18" spans="2:10" ht="19" x14ac:dyDescent="0.2">
       <c r="B18" s="79">
         <f>E4-C4</f>
-        <v>9.7500000000000031E-2</v>
+        <v>0.33000000000000007</v>
       </c>
       <c r="C18" s="80">
         <f>1-B18</f>
-        <v>0.90249999999999997</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="D18" s="80">
         <f>C18*D4</f>
-        <v>0.8491622499999999</v>
+        <v>0.45492999999999989</v>
       </c>
       <c r="E18" s="81">
         <f>D20/C20</f>
-        <v>0.89628335684062055</v>
+        <v>0.77560389610389602</v>
       </c>
       <c r="G18" s="59">
         <f>D5</f>
@@ -7278,7 +7256,7 @@
       </c>
       <c r="H18" s="55">
         <f>D4</f>
-        <v>0.94089999999999996</v>
+        <v>0.67899999999999994</v>
       </c>
       <c r="I18" s="55">
         <f>$C$8</f>
@@ -7309,7 +7287,7 @@
       </c>
       <c r="H19" s="61">
         <f>E4-D4</f>
-        <v>5.9100000000000041E-2</v>
+        <v>0.22100000000000009</v>
       </c>
       <c r="I19" s="61">
         <v>1.01</v>
@@ -7323,11 +7301,11 @@
       <c r="B20" s="73"/>
       <c r="C20" s="74">
         <f>SUM(C18:C19)</f>
-        <v>1.7725</v>
+        <v>1.54</v>
       </c>
       <c r="D20" s="74">
         <f>SUM(D18:D19)</f>
-        <v>1.5886622499999998</v>
+        <v>1.1944299999999999</v>
       </c>
       <c r="E20" s="62"/>
     </row>
@@ -7509,11 +7487,11 @@
       </c>
       <c r="J3">
         <f>Threats!B13</f>
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="K3">
         <f>Threats!C13</f>
-        <v>0.97</v>
+        <v>0.7</v>
       </c>
       <c r="L3">
         <f>Results!C5</f>
@@ -7529,7 +7507,7 @@
       </c>
       <c r="O3">
         <f>Threats!D13</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="P3">
         <f>MIN(Records!A10:A125)</f>
@@ -7553,11 +7531,11 @@
       </c>
       <c r="U3">
         <f>COUNT(Surveys!A15:A125)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V3">
         <f>F3-P3-R3-U3</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>